<commit_message>
Kleinere Anpassungen in Risikoanalyse
- Kopfzeile angepasst
- in Risikomatrix Diagramm und Kodierung getauscht
</commit_message>
<xml_diff>
--- a/Risikoanalayse T3.xlsx
+++ b/Risikoanalayse T3.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7980"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Risikoanalyse" sheetId="1" r:id="rId1"/>
+    <sheet name="Risikomatrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$I$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Risikoanalyse!$I$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
-  <si>
-    <t>Risiko-ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>R_01</t>
   </si>
@@ -69,9 +66,6 @@
     <t>Eintrittswahrscheinlichkeit</t>
   </si>
   <si>
-    <t>5% (Gering)</t>
-  </si>
-  <si>
     <t>Eintrittsindikator</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>Entscheidungen verzögern sich oder werden ersatzweise vom Projektleiter getroffen, wodurch Änderungswünsche aufkommen können und damit den Projektabschluss verzögern</t>
   </si>
   <si>
-    <t>10% (Gering)</t>
-  </si>
-  <si>
     <t>Fernbleiben bei vereinbarten Terminen</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>Zurückgewinnen von Teammitgliedern oder Finden von Ersatzteammitgliedern</t>
   </si>
   <si>
-    <t>15% (Mittel)</t>
-  </si>
-  <si>
     <t>Fehlen von Mitarbeitern</t>
   </si>
   <si>
@@ -147,15 +135,9 @@
     <t>(erhebliche) Verzögerungen in Arbeitspaketen</t>
   </si>
   <si>
-    <t>Gegenmaßnahmen geplant</t>
-  </si>
-  <si>
     <t>Übergabe der Arbeitspakete an andere Projektmitglieder</t>
   </si>
   <si>
-    <t>20% (Mittel)</t>
-  </si>
-  <si>
     <t>Langzeitige Krankschreibung von Projektmitgliedern</t>
   </si>
   <si>
@@ -168,9 +150,6 @@
     <t>Erstellung eines Kommunikationsplans und Forderung der Einhaltung</t>
   </si>
   <si>
-    <t>25% (Mittel)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unterschiedliche Informationsstände oder Fehlinformationen </t>
   </si>
   <si>
@@ -186,9 +165,6 @@
     <t>Verwendung von Puffern und ggf. Lösungssuche im Team</t>
   </si>
   <si>
-    <t>40% (Mittel)</t>
-  </si>
-  <si>
     <t>Berichte von Teammitgliedern oder Verzögerungen in der Umsetztung</t>
   </si>
   <si>
@@ -202,9 +178,6 @@
   </si>
   <si>
     <t>Wiederholte Statusnachfrage bei Lieferanten</t>
-  </si>
-  <si>
-    <t>60% (Mittel)</t>
   </si>
   <si>
     <t>Die Umsetzung kann nicht fortgesetzt werden, weil Komponenten fehlen</t>
@@ -522,7 +495,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$D$5</c:f>
+              <c:f>Risikomatrix!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -613,7 +586,7 @@
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Tabelle2!$B$6:$C$14</c:f>
+              <c:f>Risikomatrix!$B$6:$C$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="9"/>
                 <c:lvl>
@@ -679,7 +652,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$D$6:$D$14</c:f>
+              <c:f>Risikomatrix!$D$6:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -724,11 +697,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="159201512"/>
-        <c:axId val="389590640"/>
+        <c:axId val="313250664"/>
+        <c:axId val="313251056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="159201512"/>
+        <c:axId val="313250664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,7 +744,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389590640"/>
+        <c:crossAx val="313251056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -779,7 +752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="389590640"/>
+        <c:axId val="313251056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +803,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="159201512"/>
+        <c:crossAx val="313250664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1476,15 +1449,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>717440</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114841</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>203090</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1493,10 +1466,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="285750" y="2838450"/>
-          <a:ext cx="4794140" cy="2991391"/>
+          <a:off x="590550" y="5943600"/>
+          <a:ext cx="4794140" cy="3067049"/>
           <a:chOff x="552450" y="12011025"/>
-          <a:chExt cx="4440572" cy="3560986"/>
+          <a:chExt cx="4440572" cy="3651050"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -1507,9 +1480,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="552450" y="12334875"/>
-            <a:ext cx="4440572" cy="3237136"/>
+            <a:ext cx="4440572" cy="3327200"/>
             <a:chOff x="428625" y="15268575"/>
-            <a:chExt cx="4440572" cy="3237136"/>
+            <a:chExt cx="4440572" cy="3327200"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:grpSp>
@@ -2285,8 +2258,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3895725" y="18068925"/>
-              <a:ext cx="973472" cy="436786"/>
+              <a:off x="3895725" y="18068924"/>
+              <a:ext cx="973472" cy="526851"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2309,7 +2282,7 @@
           </xdr:style>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
+              <a:noAutofit/>
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
@@ -2376,15 +2349,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2717,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="400" workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="400" workbookViewId="0">
+      <selection sqref="A1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,63 +2714,63 @@
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="J4" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5" s="7">
         <v>4</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J5" s="14">
         <v>0.05</v>
@@ -2805,31 +2778,31 @@
     </row>
     <row r="6" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="H6" s="8">
         <v>3</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="15">
         <v>0.1</v>
@@ -2837,31 +2810,31 @@
     </row>
     <row r="7" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="H7" s="7">
         <v>4</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7" s="14">
         <v>0.05</v>
@@ -2869,31 +2842,31 @@
     </row>
     <row r="8" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H8" s="8">
         <v>2</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J8" s="15">
         <v>0.15</v>
@@ -2901,31 +2874,31 @@
     </row>
     <row r="9" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J9" s="14">
         <v>0.2</v>
@@ -2933,31 +2906,31 @@
     </row>
     <row r="10" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H10" s="8">
         <v>2</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J10" s="15">
         <v>0.25</v>
@@ -2965,31 +2938,31 @@
     </row>
     <row r="11" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H11" s="7">
         <v>4</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J11" s="14">
         <v>0.4</v>
@@ -2997,31 +2970,31 @@
     </row>
     <row r="12" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H12" s="8">
         <v>5</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J12" s="15">
         <v>0.6</v>
@@ -3062,7 +3035,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;CRisikoanalyse</oddHeader>
+    <oddHeader>&amp;LT3&amp;CRisikoanalyse</oddHeader>
     <oddFooter>&amp;RSeite &amp;P von &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
@@ -3073,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3085,120 +3058,120 @@
   <sheetData>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D6" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B6,Tabelle1!$J$5:$J$12,"&lt;15%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B6,Risikoanalyse!$J$5:$J$12,"&lt;15%")</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D7" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B7,Tabelle1!$J$5:$J$12,"&gt;=15%")-COUNTIFS(Tabelle1!$I$5:$I$12,B7,Tabelle1!$J$5:$J$12,"&gt;60%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B7,Risikoanalyse!$J$5:$J$12,"&gt;=15%")-COUNTIFS(Risikoanalyse!$I$5:$I$12,B7,Risikoanalyse!$J$5:$J$12,"&gt;60%")</f>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D8" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B8,Tabelle1!$J$5:$J$12,"&gt;60%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B8,Risikoanalyse!$J$5:$J$12,"&gt;60%")</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D9" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B9,Tabelle1!$J$5:$J$12,"&lt;15%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B9,Risikoanalyse!$J$5:$J$12,"&lt;15%")</f>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D10" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B10,Tabelle1!$J$5:$J$12,"&gt;=15%")-COUNTIFS(Tabelle1!$I$5:$I$12,B10,Tabelle1!$J$5:$J$12,"&gt;60%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B10,Risikoanalyse!$J$5:$J$12,"&gt;=15%")-COUNTIFS(Risikoanalyse!$I$5:$I$12,B10,Risikoanalyse!$J$5:$J$12,"&gt;60%")</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D11" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B11,Tabelle1!$J$5:$J$12,"&gt;60%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B11,Risikoanalyse!$J$5:$J$12,"&gt;60%")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D12" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B12,Tabelle1!$J$5:$J$12,"&lt;15%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B12,Risikoanalyse!$J$5:$J$12,"&lt;15%")</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B13,Tabelle1!$J$5:$J$12,"&gt;=15%")-COUNTIFS(Tabelle1!$I$5:$I$12,B13,Tabelle1!$J$5:$J$12,"&gt;60%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B13,Risikoanalyse!$J$5:$J$12,"&gt;=15%")-COUNTIFS(Risikoanalyse!$I$5:$I$12,B13,Risikoanalyse!$J$5:$J$12,"&gt;60%")</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D14" s="16">
-        <f>COUNTIFS(Tabelle1!$I$5:$I$12,B14,Tabelle1!$J$5:$J$12,"&gt;60%")</f>
+        <f>COUNTIFS(Risikoanalyse!$I$5:$I$12,B14,Risikoanalyse!$J$5:$J$12,"&gt;60%")</f>
         <v>0</v>
       </c>
     </row>
@@ -3206,7 +3179,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;CRisikomatrix</oddHeader>
+    <oddHeader>&amp;LT3&amp;CRisikomatrix</oddHeader>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>